<commit_message>
Ajout de la sauvegarde databse pour entraineur
</commit_message>
<xml_diff>
--- a/WpfTennis/WpfTennis/bin/Debug/Les Lillas/FichierAdministrationLes Lillas.xlsx
+++ b/WpfTennis/WpfTennis/bin/Debug/Les Lillas/FichierAdministrationLes Lillas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sacha\Documents\Informatique\Informatique C#\Esilv_année_2019\Wpf_Tennis\WpfTennis\WpfTennis\bin\Debug\Les Lillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sacha\Documents\Informatique\GitHub\Wpf_Projet_Tennis_Final\WpfTennis\WpfTennis\bin\Debug\Les Lillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90D9F67-D74B-4D2C-ADF5-A38F55D6D255}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE92F6E3-4A70-4739-BF94-398B13B9BD0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="0" windowWidth="17280" windowHeight="7692" xr2:uid="{EBC8A776-919C-4A83-AA6F-C896E080C6C2}"/>
+    <workbookView xWindow="5280" yWindow="2232" windowWidth="16872" windowHeight="9060" xr2:uid="{EBC8A776-919C-4A83-AA6F-C896E080C6C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>

</xml_diff>